<commit_message>
Falta Datos del comprador y del producto
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jersondavidsanchez/PycharmProjects/web-cafiagro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f15af156e68905c6/Escritorio/Cafiagro Progra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56933822-B321-E740-870E-A9DF515F0D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{56933822-B321-E740-870E-A9DF515F0D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B401564-1E3C-4C0F-ACF9-327F65FF8352}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="1200" windowWidth="24240" windowHeight="15540" xr2:uid="{248F28A4-9119-4F58-BF02-7C88DEE08585}"/>
+    <workbookView xWindow="390" yWindow="1200" windowWidth="16200" windowHeight="10060" xr2:uid="{248F28A4-9119-4F58-BF02-7C88DEE08585}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -402,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D46B30-E479-411E-9A3E-33B1E574F99E}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12345</v>
       </c>
@@ -430,6 +430,17 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>13123</v>
+      </c>
+      <c r="B3">
+        <v>2412</v>
+      </c>
+      <c r="C3">
+        <v>241241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>